<commit_message>
bug fixes in api
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testScript-Api.xlsx
+++ b/Web/coyni/resources/testScript-Api.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebAutomation\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD80C4D-3AFA-4B28-85B1-4255BC81595A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67652C1C-722F-43D1-8A33-6C0435A99668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C69601D5-11F0-4855-BF49-0402CA84EEE6}"/>
+    <workbookView xWindow="4065" yWindow="4065" windowWidth="10455" windowHeight="9180" xr2:uid="{C69601D5-11F0-4855-BF49-0402CA84EEE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="300">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -782,34 +782,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>coyni.apibusiness.tests.BusinessProfileTest,
-testEditEmailAddressWithInvalidAuthy,
--pemail,
--pemailHeading1,
--pemailHeading2,
--pchar,
--ppin,
--perrMessage,
--pvalidPin,
--penterEmail,
--pemailHeading,
--pemailAddressHeading,
--pnewEmailPopUp,
--pnewEmail</t>
-  </si>
-  <si>
     <t>testEditEmailAddressInvalidData</t>
-  </si>
-  <si>
-    <t>coyni.apibusiness.tests.BusinessProfileTest,
-testEditEmailAddressInvalidData,
--pemail,
--pcode,
--pemailAddressHeading,
--pnewEmail,
--pcolour,
--pelementName,
--perrMessage</t>
   </si>
   <si>
     <t>testGetSmsCodeVerificationEmailAddress</t>
@@ -968,19 +941,7 @@
     <t>testData_Api.xlsx,PaymentMethods</t>
   </si>
   <si>
-    <t>testTokenWalletBuyTokensBuyTokensBankAccount</t>
-  </si>
-  <si>
     <t>testData_Api.xlsx,BuyTokens</t>
-  </si>
-  <si>
-    <t>coyni.apibusiness.tests.TokenWalletTest,
-testTokenWalletBuyTokensBankAccount,
--pheading,
--psubHeading,
--pamount,
--pcode,
--ppreviewHeading</t>
   </si>
   <si>
     <t>testBusinenssSettingsAddSignetAccount</t>
@@ -1819,6 +1780,36 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>coyni.apibusiness.tests.BusinessProfileTest,
+testEditEmailAddressWithInvalidAuthy,
+-pemail1,
+-pemailHeading1,
+-pemailHeading2,
+-pchar,
+-ppin,
+-perrMessage,
+-pvalidPin,
+-penterEmail,
+-pemailHeading,
+-pemailAddressHeading,
+-pnewEmailPopUp,
+-pnewEmail</t>
+  </si>
+  <si>
+    <t>coyni.apibusiness.tests.BusinessProfileTest,
+testEditEmailAddressInvalidData,
+-pemail1,
+-pcode,
+-pemailAddressHeading,
+-pnewEmail,
+-pcolour,
+-pelementName,
+-perrMessage</t>
   </si>
 </sst>
 </file>
@@ -2296,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DE51BD-94A5-42A8-A4AC-1B2005B22766}">
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2340,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>10</v>
@@ -2378,7 +2369,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>10</v>
@@ -2407,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>10</v>
@@ -2436,7 +2427,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>10</v>
@@ -2465,7 +2456,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>10</v>
@@ -2494,7 +2485,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
@@ -2523,7 +2514,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>10</v>
@@ -2552,7 +2543,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -2581,7 +2572,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>10</v>
@@ -2610,7 +2601,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>10</v>
@@ -2639,7 +2630,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>10</v>
@@ -2668,7 +2659,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>10</v>
@@ -2697,7 +2688,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>10</v>
@@ -2726,7 +2717,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>10</v>
@@ -2755,7 +2746,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>10</v>
@@ -2784,7 +2775,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>10</v>
@@ -2813,7 +2804,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>10</v>
@@ -2842,7 +2833,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>10</v>
@@ -2871,7 +2862,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>10</v>
@@ -2900,7 +2891,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>55</v>
@@ -2926,7 +2917,7 @@
         <v>57</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>55</v>
@@ -2938,7 +2929,7 @@
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>56</v>
@@ -2952,7 +2943,7 @@
         <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>55</v>
@@ -2978,7 +2969,7 @@
         <v>60</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>55</v>
@@ -3004,7 +2995,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>55</v>
@@ -3030,13 +3021,13 @@
         <v>63</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>12</v>
@@ -3056,7 +3047,7 @@
         <v>66</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>64</v>
@@ -3082,7 +3073,7 @@
         <v>67</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>64</v>
@@ -3108,7 +3099,7 @@
         <v>69</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>64</v>
@@ -3134,7 +3125,7 @@
         <v>70</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>64</v>
@@ -3160,7 +3151,7 @@
         <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>72</v>
@@ -3186,7 +3177,7 @@
         <v>74</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>72</v>
@@ -3212,7 +3203,7 @@
         <v>75</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>72</v>
@@ -3224,7 +3215,7 @@
         <v>12</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>62</v>
+        <v>297</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>73</v>
@@ -3238,7 +3229,7 @@
         <v>76</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>72</v>
@@ -3264,7 +3255,7 @@
         <v>77</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C35" s="25" t="s">
         <v>72</v>
@@ -3290,7 +3281,7 @@
         <v>78</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>72</v>
@@ -3316,7 +3307,7 @@
         <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>80</v>
@@ -3345,7 +3336,7 @@
         <v>82</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>80</v>
@@ -3374,7 +3365,7 @@
         <v>84</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>80</v>
@@ -3403,7 +3394,7 @@
         <v>104</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>105</v>
@@ -3432,7 +3423,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C41" s="25" t="s">
         <v>105</v>
@@ -3461,7 +3452,7 @@
         <v>110</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>105</v>
@@ -3470,7 +3461,7 @@
         <v>17</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>58</v>
@@ -3482,15 +3473,15 @@
         <v>14</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>112</v>
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>105</v>
@@ -3499,7 +3490,7 @@
         <v>17</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>62</v>
@@ -3511,15 +3502,15 @@
         <v>14</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>114</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>105</v>
@@ -3540,15 +3531,15 @@
         <v>14</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>105</v>
@@ -3569,47 +3560,47 @@
         <v>14</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="H46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>11</v>
@@ -3621,24 +3612,24 @@
         <v>12</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="280.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>17</v>
@@ -3650,24 +3641,24 @@
         <v>68</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>17</v>
@@ -3679,24 +3670,24 @@
         <v>12</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>17</v>
@@ -3708,24 +3699,24 @@
         <v>12</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>17</v>
@@ -3737,24 +3728,24 @@
         <v>12</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>17</v>
@@ -3766,24 +3757,24 @@
         <v>68</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>17</v>
@@ -3795,24 +3786,24 @@
         <v>12</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>17</v>
@@ -3824,24 +3815,24 @@
         <v>1</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>17</v>
@@ -3853,24 +3844,24 @@
         <v>1</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>11</v>
@@ -3882,401 +3873,401 @@
         <v>12</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="24" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="H57" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I57" s="23" t="s">
+    </row>
+    <row r="58" spans="1:9" s="24" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A58" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="23" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+    <row r="59" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I58" s="10" t="s">
+      <c r="B59" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" s="24" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+      <c r="D59" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="H59" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C60" s="11" t="s">
+    </row>
+    <row r="61" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D60" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I60" s="6" t="s">
+      <c r="B61" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+    <row r="62" spans="1:9" s="24" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A62" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="6" t="s">
+      <c r="B62" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H62" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="B63" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I62" s="6" t="s">
+    </row>
+    <row r="64" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" s="24" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A63" s="21" t="s">
+      <c r="B64" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="H63" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I63" s="23" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+    </row>
+    <row r="65" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I64" s="6" t="s">
+      <c r="B65" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="6" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I66" s="6" t="s">
+      <c r="B67" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I67" s="16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+    <row r="68" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I67" s="6" t="s">
+      <c r="B68" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="D68" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H68" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B68" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I68" s="16" t="s">
+      <c r="I68" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+    <row r="69" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C69" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I69" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>11</v>
@@ -4288,24 +4279,24 @@
         <v>12</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>11</v>
@@ -4317,25 +4308,25 @@
         <v>12</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I71" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>169</v>
-      </c>
       <c r="D72" s="11" t="s">
         <v>11</v>
       </c>
@@ -4346,53 +4337,53 @@
         <v>12</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H73" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="I73" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I73" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>11</v>
@@ -4404,123 +4395,123 @@
         <v>12</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H74" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H74" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="4" t="s">
         <v>183</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>121</v>
+        <v>294</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
         <v>187</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C76" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G76" s="4" t="s">
+      <c r="D76" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" s="15" t="s">
         <v>189</v>
       </c>
+      <c r="G76" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="H76" s="6" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D77" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D78" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E77" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
+      <c r="E78" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>12</v>
-      </c>
       <c r="G78" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>14</v>
@@ -4534,475 +4525,475 @@
         <v>198</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D79" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G80" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I80" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" s="14" t="s">
         <v>204</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F81" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H81" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I81" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H82" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="14" t="s">
+      <c r="B84" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="14" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+    <row r="85" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F83" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I83" s="14" t="s">
+      <c r="B85" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="14" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F84" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F85" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I85" s="14" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B86" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F86" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H86" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I86" s="14" t="s">
+      <c r="B87" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+    <row r="88" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A88" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F87" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="14" t="s">
+      <c r="B88" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+    <row r="89" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C88" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F88" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H88" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="6" t="s">
+      <c r="B89" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" s="14" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+    <row r="90" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A90" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E89" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F89" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G89" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I89" s="14" t="s">
+      <c r="B90" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
+    <row r="91" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B90" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F90" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H90" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I90" s="14" t="s">
+      <c r="B91" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="14" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+    <row r="92" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F91" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="H91" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I91" s="14" t="s">
+      <c r="B92" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
+      <c r="D92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="4">
+        <v>1</v>
+      </c>
+      <c r="F92" s="4">
+        <v>1</v>
+      </c>
+      <c r="G92" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="D92" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F92" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" s="11" t="s">
-        <v>194</v>
-      </c>
       <c r="H92" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I92" s="14" t="s">
+      <c r="I92" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C93" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C93" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E93" s="4">
-        <v>1</v>
-      </c>
-      <c r="F93" s="4">
-        <v>1</v>
-      </c>
-      <c r="G93" s="12" t="s">
+      <c r="D93" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I93" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="H93" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I93" s="6" t="s">
+    </row>
+    <row r="94" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
+      <c r="B94" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C94" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C94" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D94" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E94" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F94" s="13" t="s">
+      <c r="D94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I94" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C95" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C95" s="18" t="s">
-        <v>235</v>
-      </c>
       <c r="D95" s="4" t="s">
         <v>11</v>
       </c>
@@ -5013,24 +5004,24 @@
         <v>12</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I95" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>237</v>
-      </c>
       <c r="B96" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>11</v>
@@ -5042,24 +5033,24 @@
         <v>12</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I96" s="14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>11</v>
@@ -5071,53 +5062,53 @@
         <v>12</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I97" s="14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>12</v>
+        <v>241</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I98" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>17</v>
@@ -5126,85 +5117,85 @@
         <v>12</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>245</v>
+        <v>12</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H99" s="6" t="s">
         <v>100</v>
       </c>
       <c r="I99" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C100" s="18" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
+      <c r="D100" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H100" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="B100" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C100" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H100" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I100" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H101" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C101" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D101" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E101" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F101" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="H101" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I101" s="6" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D102" s="18" t="s">
         <v>11</v>
@@ -5216,111 +5207,111 @@
         <v>12</v>
       </c>
       <c r="G102" s="18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H102" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I102" s="6" t="s">
-        <v>253</v>
+      <c r="I102" s="14" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H103" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B103" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C103" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D103" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E103" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="H103" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I103" s="14" t="s">
+      <c r="B104" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C104" s="18" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="D104" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H104" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D104" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E104" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F104" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="H104" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I104" s="14" t="s">
+    </row>
+    <row r="105" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A105" s="11" t="s">
+      <c r="B105" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H105" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C105" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="D105" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I105" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D106" s="18" t="s">
         <v>11</v>
@@ -5332,128 +5323,128 @@
         <v>12</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H106" s="14" t="s">
         <v>14</v>
       </c>
       <c r="I106" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H107" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A108" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="B107" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C107" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="D107" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E107" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F107" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="H107" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I107" s="14" t="s">
+      <c r="B108" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C108" s="18" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
+      <c r="D108" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H108" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="D108" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E108" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F108" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="H108" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I108" s="14" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C109" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D109" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E109" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="H109" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I109" s="14" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D110" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E110" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="H110" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I110" s="14" t="s">
+      <c r="H110" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" s="6" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5462,39 +5453,39 @@
         <v>272</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C111" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" s="6" t="s">
         <v>273</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E111" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="H111" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I111" s="6" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>11</v>
@@ -5506,137 +5497,137 @@
         <v>12</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H112" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I112" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="B113" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C113" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E113" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="11" t="s">
-        <v>274</v>
-      </c>
       <c r="H113" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I113" s="6" t="s">
+      <c r="I113" s="20" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A114" s="11" t="s">
+      <c r="A114" s="12" t="s">
         <v>280</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C114" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="H114" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I114" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="D114" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F114" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="11" t="s">
+    </row>
+    <row r="115" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="H114" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I114" s="20" t="s">
+      <c r="B115" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C115" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I115" s="20" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
+    <row r="116" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A116" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="B115" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F115" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="H115" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I115" s="20" t="s">
+      <c r="B116" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C116" s="11" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
+      <c r="D116" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="11" t="s">
-        <v>282</v>
-      </c>
       <c r="H116" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I116" s="20" t="s">
+      <c r="I116" s="14" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="11" t="s">
         <v>288</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C117" s="11" t="s">
         <v>289</v>
@@ -5656,7 +5647,7 @@
       <c r="H117" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I117" s="14" t="s">
+      <c r="I117" s="20" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5665,61 +5656,32 @@
         <v>292</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C118" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F118" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I118" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E118" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F118" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="H118" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I118" s="20" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A119" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E119" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="H119" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I119" s="20" t="s">
-        <v>297</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I119" xr:uid="{17DE51BD-94A5-42A8-A4AC-1B2005B22766}"/>
+  <autoFilter ref="A1:I118" xr:uid="{17DE51BD-94A5-42A8-A4AC-1B2005B22766}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified test methods in API Business
</commit_message>
<xml_diff>
--- a/Web/coyni/resources/testScript-Api.xlsx
+++ b/Web/coyni/resources/testScript-Api.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\March17Automation\coyni-automation\Web\coyni\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\28-03-2023\coyni-automation\Web\coyni\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A056F1C-E40D-480F-9CA7-78FBD5AD101C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685B5269-3039-47F4-95AC-141C3B8AB1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C69601D5-11F0-4855-BF49-0402CA84EEE6}"/>
   </bookViews>
@@ -783,17 +783,6 @@
     <t>testTokenWalletWithdrawToUsdViaInstantPay</t>
   </si>
   <si>
-    <t>coyni.apibusiness.tests.TokenWalletTest,
-testTokenWalletWithdrawToUsdViaInstantPay,
--pheading,
--plast4digits,
--pinstantPayHeading,
--pamount,
--pmessage,
--ptransactionInProgHdg,
--pcode</t>
-  </si>
-  <si>
     <t>testWithdrawToUSDViaInstantPayWithInvalidDetails</t>
   </si>
   <si>
@@ -962,29 +951,10 @@
     <t>testData_Api.xlsx,AccountLimits</t>
   </si>
   <si>
-    <t>testBusinessSettingsNoTeamMember</t>
-  </si>
-  <si>
     <t>testData_Api.xlsx,Team</t>
   </si>
   <si>
     <t>testBusinessSettingsAddTeamMember</t>
-  </si>
-  <si>
-    <t>coyni.apibusiness.tests.BusinessSettingsTest,
-testBusinessSettingsAddTeamMember,
--paddTeamHeading,
--pfirstName,
--plastName,
--pemaildet,
--pphone,
--pcustomHeading,
--proleName,
--pmessage,
--pexpHeading,
--poption,
--peleName,
--ptitle</t>
   </si>
   <si>
     <t>testBusinessSettingsTeamFilters</t>
@@ -1385,17 +1355,6 @@
 -paccountID,
 -paccountStatus
 </t>
-  </si>
-  <si>
-    <t>coyni.apibusiness.tests.BusinessSettingsTest,_x000D_
-testBusinessSettingsAddExternalBank,_x000D_
--pexpBankName,_x000D_
--pexpUserName,_x000D_
--pexpPassword,_x000D_
--proutingNumber,_x000D_
--pconfirmRoutingNumber,_x000D_
--paccountNumber,_x000D_
--pconfirmAccountNumber</t>
   </si>
   <si>
     <t>coyni.apibusiness.tests.BusinessSettingsTest,_x000D_
@@ -1752,11 +1711,6 @@
   </si>
   <si>
     <t>coyni.apibusiness.tests.BusinessSettingsTest,
-testBusinessSettingsNoTeamMember,
--pheading</t>
-  </si>
-  <si>
-    <t>coyni.apibusiness.tests.BusinessSettingsTest,
 testBusinessSettingsTeamFilters,
 -pheading</t>
   </si>
@@ -1837,6 +1791,57 @@
 -pipAddress,
 -pipDescription,
 -psuccessHeading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coyni.apibusiness.tests.TokenWalletTest,
+testTokenWalletWithdrawToUsdViaInstantPay,
+-pheading,
+-plast4digits,
+-pinstantPayHeading,
+-pamount,
+-pmessage,
+-ptransactionInProgHdg,
+-pcode,
+-ploginHeading,
+-ploginDescription,
+-pemail,
+-ppassword,
+-pauthyHeading,
+-pauthyDescription
+</t>
+  </si>
+  <si>
+    <t>coyni.apibusiness.tests.BusinessSettingsTest,
+testBusinessSettingsAddTeamMember,
+-paddTeamHeading,
+-pfirstName,
+-plastName,
+-pemaildet,
+-pphone,
+-pcustomHeading,
+-proleName,
+-pmessage,
+-pexpHeading,
+-poption,
+-peleName,
+-ptoastTitle,
+-ptoastMessage,
+-pmessage</t>
+  </si>
+  <si>
+    <t>testTeamFilters</t>
+  </si>
+  <si>
+    <t>coyni.apibusiness.tests.BusinessSettingsTest,
+testTeamFilters,
+-pheading</t>
+  </si>
+  <si>
+    <t>coyni.apibusiness.tests.BusinessSettingsTest,
+testBusinessSettingsAddExternalBank,
+-pexpBankName,
+-pexpUserName,
+-pexpPassword</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1999,12 +2004,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2017,6 +2016,33 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2333,8 +2359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DE51BD-94A5-42A8-A4AC-1B2005B22766}">
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,6 +2374,7 @@
     <col min="7" max="7" width="41" customWidth="1"/>
     <col min="8" max="8" width="40.140625" customWidth="1"/>
     <col min="9" max="9" width="84.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2384,7 +2411,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>34</v>
@@ -2411,7 +2438,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>34</v>
@@ -2438,7 +2465,7 @@
         <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>34</v>
@@ -2465,7 +2492,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>34</v>
@@ -2492,7 +2519,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>43</v>
@@ -2519,7 +2546,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>43</v>
@@ -2546,7 +2573,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>43</v>
@@ -2573,7 +2600,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>43</v>
@@ -2600,7 +2627,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>43</v>
@@ -2627,7 +2654,7 @@
         <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>51</v>
@@ -2654,7 +2681,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>51</v>
@@ -2681,7 +2708,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>51</v>
@@ -2708,7 +2735,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>51</v>
@@ -2735,7 +2762,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>51</v>
@@ -2762,7 +2789,7 @@
         <v>53</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>51</v>
@@ -2786,13 +2813,13 @@
     </row>
     <row r="17" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>11</v>
@@ -2804,42 +2831,42 @@
         <v>12</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="270" x14ac:dyDescent="0.25">
@@ -2847,7 +2874,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -2862,10 +2889,10 @@
         <v>12</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>14</v>
@@ -2876,7 +2903,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>10</v>
@@ -2891,13 +2918,13 @@
         <v>17</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -2905,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>10</v>
@@ -2920,10 +2947,10 @@
         <v>12</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>19</v>
@@ -2934,7 +2961,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>10</v>
@@ -2949,10 +2976,10 @@
         <v>12</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>21</v>
@@ -2963,7 +2990,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>10</v>
@@ -2978,10 +3005,10 @@
         <v>12</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>23</v>
@@ -2992,7 +3019,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>10</v>
@@ -3007,13 +3034,13 @@
         <v>12</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -3021,7 +3048,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>10</v>
@@ -3036,13 +3063,13 @@
         <v>17</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="240" x14ac:dyDescent="0.25">
@@ -3050,7 +3077,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>10</v>
@@ -3065,10 +3092,10 @@
         <v>12</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>27</v>
@@ -3079,7 +3106,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>10</v>
@@ -3094,13 +3121,13 @@
         <v>12</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="315" x14ac:dyDescent="0.25">
@@ -3108,7 +3135,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>10</v>
@@ -3123,13 +3150,13 @@
         <v>12</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3137,7 +3164,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>10</v>
@@ -3152,10 +3179,10 @@
         <v>12</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>31</v>
@@ -3166,7 +3193,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>10</v>
@@ -3181,13 +3208,13 @@
         <v>12</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3195,7 +3222,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>10</v>
@@ -3210,19 +3237,19 @@
         <v>12</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -3235,7 +3262,7 @@
     <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -3248,7 +3275,7 @@
     <row r="34" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -3261,7 +3288,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -3274,7 +3301,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -3289,7 +3316,7 @@
         <v>96</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>97</v>
@@ -3318,7 +3345,7 @@
         <v>100</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>97</v>
@@ -3347,7 +3374,7 @@
         <v>102</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>97</v>
@@ -3376,7 +3403,7 @@
         <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>97</v>
@@ -3405,7 +3432,7 @@
         <v>106</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>97</v>
@@ -3423,7 +3450,7 @@
         <v>98</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>107</v>
@@ -3434,7 +3461,7 @@
         <v>108</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>97</v>
@@ -3452,7 +3479,7 @@
         <v>98</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>109</v>
@@ -3463,7 +3490,7 @@
         <v>110</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>97</v>
@@ -3481,7 +3508,7 @@
         <v>98</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>111</v>
@@ -3492,7 +3519,7 @@
         <v>112</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>97</v>
@@ -3510,21 +3537,21 @@
         <v>98</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I44" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="I44" s="29" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>11</v>
@@ -3539,10 +3566,10 @@
         <v>98</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
@@ -3550,7 +3577,7 @@
         <v>114</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>97</v>
@@ -3568,7 +3595,7 @@
         <v>98</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>115</v>
@@ -3579,7 +3606,7 @@
         <v>116</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>117</v>
@@ -3597,21 +3624,21 @@
         <v>98</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>11</v>
@@ -3626,21 +3653,21 @@
         <v>98</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>11</v>
@@ -3658,47 +3685,47 @@
         <v>77</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="26" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C50" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="19" t="s">
+      <c r="D50" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="H50" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>260</v>
+      <c r="H50" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>11</v>
@@ -3713,7 +3740,7 @@
         <v>98</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I51" s="14" t="s">
         <v>119</v>
@@ -3721,13 +3748,13 @@
     </row>
     <row r="52" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>11</v>
@@ -3745,7 +3772,7 @@
         <v>77</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3753,7 +3780,7 @@
         <v>120</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>121</v>
@@ -3771,18 +3798,18 @@
         <v>98</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>117</v>
@@ -3803,15 +3830,15 @@
         <v>13</v>
       </c>
       <c r="I54" s="18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>121</v>
@@ -3829,18 +3856,18 @@
         <v>98</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>121</v>
@@ -3858,18 +3885,18 @@
         <v>98</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="26" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>121</v>
@@ -3890,15 +3917,15 @@
         <v>77</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>121</v>
@@ -3916,21 +3943,21 @@
         <v>98</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>11</v>
@@ -3945,10 +3972,10 @@
         <v>98</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -3956,7 +3983,7 @@
         <v>122</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>121</v>
@@ -3974,18 +4001,18 @@
         <v>98</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>121</v>
@@ -4003,18 +4030,18 @@
         <v>98</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>124</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>121</v>
@@ -4032,50 +4059,50 @@
         <v>98</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="35" customFormat="1" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
-        <v>278</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="33" customFormat="1" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
+        <v>274</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C63" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H63" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I63" s="32" t="s">
         <v>130</v>
-      </c>
-      <c r="D63" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="H63" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="I63" s="34" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>11</v>
@@ -4093,18 +4120,18 @@
         <v>77</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>11</v>
@@ -4122,15 +4149,15 @@
         <v>77</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>117</v>
@@ -4151,15 +4178,15 @@
         <v>77</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>117</v>
@@ -4180,15 +4207,15 @@
         <v>77</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>117</v>
@@ -4209,18 +4236,18 @@
         <v>77</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>11</v>
@@ -4232,53 +4259,53 @@
         <v>12</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>184</v>
+      <c r="A70" s="39" t="s">
+        <v>181</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H70" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="H70" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>256</v>
+      <c r="I70" s="22" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>11</v>
@@ -4290,24 +4317,24 @@
         <v>12</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>11</v>
@@ -4319,24 +4346,24 @@
         <v>12</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H72" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>11</v>
@@ -4348,24 +4375,24 @@
         <v>12</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H73" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I73" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>11</v>
@@ -4377,24 +4404,24 @@
         <v>12</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H74" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>11</v>
@@ -4406,24 +4433,24 @@
         <v>12</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H75" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>11</v>
@@ -4435,24 +4462,24 @@
         <v>12</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H76" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I76" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>16</v>
@@ -4464,24 +4491,24 @@
         <v>47</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H77" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I77" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>11</v>
@@ -4493,53 +4520,53 @@
         <v>12</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H78" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C79" s="8" t="s">
+      <c r="D79" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="H79" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>11</v>
@@ -4551,24 +4578,24 @@
         <v>12</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H80" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I80" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>16</v>
@@ -4577,27 +4604,27 @@
         <v>12</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H81" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I81" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>11</v>
@@ -4609,24 +4636,24 @@
         <v>12</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H82" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I82" s="15" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>16</v>
@@ -4635,28 +4662,28 @@
         <v>12</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H83" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="D84" s="3" t="s">
         <v>11</v>
       </c>
@@ -4667,21 +4694,21 @@
         <v>12</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H84" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C85" s="16" t="s">
         <v>118</v>
@@ -4696,21 +4723,21 @@
         <v>12</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H85" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I85" s="10" t="s">
-        <v>253</v>
+        <v>309</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C86" s="16" t="s">
         <v>118</v>
@@ -4725,21 +4752,21 @@
         <v>12</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H86" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C87" s="16" t="s">
         <v>118</v>
@@ -4754,21 +4781,21 @@
         <v>12</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C88" s="16" t="s">
         <v>118</v>
@@ -4783,21 +4810,21 @@
         <v>12</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H88" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C89" s="16" t="s">
         <v>118</v>
@@ -4812,21 +4839,21 @@
         <v>12</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H89" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I89" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C90" s="16" t="s">
         <v>118</v>
@@ -4841,21 +4868,21 @@
         <v>12</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H90" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I90" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C91" s="16" t="s">
         <v>118</v>
@@ -4870,21 +4897,21 @@
         <v>12</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I91" s="18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C92" s="16" t="s">
         <v>118</v>
@@ -4896,24 +4923,24 @@
         <v>12</v>
       </c>
       <c r="F92" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G92" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="H92" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I92" s="18" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C93" s="16" t="s">
         <v>118</v>
@@ -4928,21 +4955,21 @@
         <v>12</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H93" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I93" s="18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C94" s="16" t="s">
         <v>118</v>
@@ -4957,24 +4984,24 @@
         <v>12</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H94" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D95" s="16" t="s">
         <v>11</v>
@@ -4986,24 +5013,24 @@
         <v>12</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H95" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I95" s="18" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>11</v>
@@ -5015,25 +5042,25 @@
         <v>1</v>
       </c>
       <c r="G96" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H96" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B97" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C97" s="16" t="s">
-        <v>162</v>
-      </c>
       <c r="D97" s="16" t="s">
         <v>11</v>
       </c>
@@ -5044,25 +5071,25 @@
         <v>12</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H97" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I97" s="18" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C98" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C98" s="23" t="s">
-        <v>164</v>
-      </c>
       <c r="D98" s="8" t="s">
         <v>11</v>
       </c>
@@ -5073,24 +5100,24 @@
         <v>12</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H98" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I98" s="10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>11</v>
@@ -5102,24 +5129,24 @@
         <v>12</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H99" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="I99" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>11</v>
@@ -5131,24 +5158,24 @@
         <v>12</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H100" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I100" s="18" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>169</v>
+        <v>307</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>11</v>
@@ -5160,24 +5187,24 @@
         <v>12</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H101" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I101" s="18" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>16</v>
@@ -5186,27 +5213,27 @@
         <v>12</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H102" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I102" s="18" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>16</v>
@@ -5218,24 +5245,24 @@
         <v>12</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H103" s="10" t="s">
         <v>77</v>
       </c>
       <c r="I103" s="18" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D104" s="23" t="s">
         <v>11</v>
@@ -5247,53 +5274,53 @@
         <v>12</v>
       </c>
       <c r="G104" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H104" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I104" s="18" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>175</v>
+      <c r="A105" s="34" t="s">
+        <v>172</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C105" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="D105" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F105" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="H105" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C105" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D105" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="H105" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I105" s="18" t="s">
-        <v>309</v>
+      <c r="I105" s="38" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D106" s="23" t="s">
         <v>11</v>
@@ -5305,24 +5332,24 @@
         <v>12</v>
       </c>
       <c r="G106" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H106" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I106" s="18" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D107" s="23" t="s">
         <v>11</v>
@@ -5334,24 +5361,24 @@
         <v>12</v>
       </c>
       <c r="G107" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H107" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I107" s="18" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A108" s="28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D108" s="23" t="s">
         <v>11</v>
@@ -5363,53 +5390,53 @@
         <v>12</v>
       </c>
       <c r="G108" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H108" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I108" s="18" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>179</v>
+      <c r="A109" s="39" t="s">
+        <v>176</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C109" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="D109" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E109" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="H109" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C109" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D109" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="H109" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I109" s="31" t="s">
-        <v>255</v>
+      <c r="I109" s="38" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D110" s="23" t="s">
         <v>11</v>
@@ -5421,13 +5448,13 @@
         <v>12</v>
       </c>
       <c r="G110" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H110" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I110" s="18" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -5435,7 +5462,7 @@
         <v>81</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>82</v>
@@ -5464,7 +5491,7 @@
         <v>85</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>82</v>
@@ -5493,7 +5520,7 @@
         <v>87</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>82</v>
@@ -5522,7 +5549,7 @@
         <v>90</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>82</v>
@@ -5551,7 +5578,7 @@
         <v>92</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>82</v>
@@ -5580,7 +5607,7 @@
         <v>94</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>82</v>
@@ -5606,10 +5633,10 @@
     </row>
     <row r="117" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>82</v>
@@ -5630,15 +5657,15 @@
         <v>13</v>
       </c>
       <c r="I117" s="10" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>82</v>
@@ -5659,15 +5686,15 @@
         <v>13</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>82</v>
@@ -5688,18 +5715,18 @@
         <v>13</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>11</v>
@@ -5711,24 +5738,24 @@
         <v>12</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H120" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I120" s="25" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>11</v>
@@ -5740,24 +5767,24 @@
         <v>12</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H121" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I121" s="25" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>11</v>
@@ -5769,13 +5796,13 @@
         <v>12</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H122" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I122" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -5783,7 +5810,7 @@
         <v>57</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>58</v>
@@ -5812,7 +5839,7 @@
         <v>60</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>58</v>
@@ -5841,7 +5868,7 @@
         <v>62</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>58</v>

</xml_diff>